<commit_message>
Update [User Class] seuccess !!
</commit_message>
<xml_diff>
--- a/build/classes/db/BookingStock.xlsx
+++ b/build/classes/db/BookingStock.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="65">
   <si>
     <t>Booking ID</t>
   </si>
@@ -123,6 +123,90 @@
   </si>
   <si>
     <t>23-05-2020 02:05:02</t>
+  </si>
+  <si>
+    <t>1255</t>
+  </si>
+  <si>
+    <t>Delux</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>23-05-2020 02:05:36</t>
+  </si>
+  <si>
+    <t>1204</t>
+  </si>
+  <si>
+    <t>23-14-2020 02:14:17</t>
+  </si>
+  <si>
+    <t>1905</t>
+  </si>
+  <si>
+    <t>2020-04-15</t>
+  </si>
+  <si>
+    <t>2020-04-18</t>
+  </si>
+  <si>
+    <t>23-15-2020 02:15:44</t>
+  </si>
+  <si>
+    <t>1036</t>
+  </si>
+  <si>
+    <t>2020-04-25</t>
+  </si>
+  <si>
+    <t>23-18-2020 02:18:16</t>
+  </si>
+  <si>
+    <t>1660</t>
+  </si>
+  <si>
+    <t>2020-05-05</t>
+  </si>
+  <si>
+    <t>23-19-2020 02:19:16</t>
+  </si>
+  <si>
+    <t>1824</t>
+  </si>
+  <si>
+    <t>2020-04-27</t>
+  </si>
+  <si>
+    <t>23-20-2020 02:20:36</t>
+  </si>
+  <si>
+    <t>1508</t>
+  </si>
+  <si>
+    <t>2020-04-29</t>
+  </si>
+  <si>
+    <t>23-20-2020 02:20:50</t>
+  </si>
+  <si>
+    <t>1083</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>23-30-2020 02:30:20</t>
+  </si>
+  <si>
+    <t>1726</t>
+  </si>
+  <si>
+    <t>2020-05-03</t>
+  </si>
+  <si>
+    <t>23-37-2020 02:37:14</t>
   </si>
 </sst>
 </file>
@@ -167,7 +251,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -378,6 +462,429 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="n">
+        <v>11700.0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="n">
+        <v>14400.0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" t="n">
+        <v>14400.0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" t="n">
+        <v>19500.0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" t="n">
+        <v>15600.0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" t="n">
+        <v>9600.0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="n">
+        <v>17250.0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
OOP Presentation [Last Commit]
</commit_message>
<xml_diff>
--- a/build/classes/db/BookingStock.xlsx
+++ b/build/classes/db/BookingStock.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="69">
   <si>
     <t>Booking ID</t>
   </si>
@@ -128,130 +128,97 @@
     <t>23-04-2020 04:01:00</t>
   </si>
   <si>
-    <t>1357</t>
+    <t>1440</t>
+  </si>
+  <si>
+    <t>2020-04-29</t>
+  </si>
+  <si>
+    <t>2020-05-02</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2850.0</t>
+  </si>
+  <si>
+    <t>23-04-2020 04:01:23</t>
+  </si>
+  <si>
+    <t>1035</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>1440</t>
-  </si>
-  <si>
-    <t>2020-04-29</t>
-  </si>
-  <si>
-    <t>2020-05-02</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2850.0</t>
-  </si>
-  <si>
-    <t>23-04-2020 04:01:23</t>
-  </si>
-  <si>
-    <t>1035</t>
-  </si>
-  <si>
-    <t>1028</t>
-  </si>
-  <si>
-    <t>nnn   nnn</t>
+    <t>1248</t>
+  </si>
+  <si>
+    <t>2020-04-28</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>14100.0</t>
+  </si>
+  <si>
+    <t>24-04-2020 11:30:40</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>2020-04-30</t>
+  </si>
+  <si>
+    <t>2020-05-03</t>
+  </si>
+  <si>
+    <t>9900.0</t>
+  </si>
+  <si>
+    <t>24-04-2020 11:57:44</t>
+  </si>
+  <si>
+    <t>1062</t>
+  </si>
+  <si>
+    <t>6600.0</t>
+  </si>
+  <si>
+    <t>24-04-2020 12:10:54</t>
+  </si>
+  <si>
+    <t>1041</t>
+  </si>
+  <si>
+    <t>24300.0</t>
+  </si>
+  <si>
+    <t>24-04-2020 12:48:27</t>
+  </si>
+  <si>
+    <t>1719</t>
+  </si>
+  <si>
+    <t>1545</t>
   </si>
   <si>
     <t>2020-04-25</t>
   </si>
   <si>
-    <t>9600.0</t>
-  </si>
-  <si>
-    <t>23-04-2020 05:32:51</t>
-  </si>
-  <si>
-    <t>1921</t>
-  </si>
-  <si>
-    <t>2020-04-30</t>
-  </si>
-  <si>
-    <t>2020-05-04</t>
-  </si>
-  <si>
-    <t>8000.0</t>
-  </si>
-  <si>
-    <t>24-04-2020 02:33:41</t>
-  </si>
-  <si>
-    <t>1055</t>
-  </si>
-  <si>
-    <t>2020-05-03</t>
-  </si>
-  <si>
-    <t>6000.0</t>
-  </si>
-  <si>
-    <t>24-04-2020 04:03:43</t>
-  </si>
-  <si>
-    <t>1889</t>
-  </si>
-  <si>
-    <t>Junior Suite</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>36000.0</t>
-  </si>
-  <si>
-    <t>24-04-2020 04:26:22</t>
-  </si>
-  <si>
-    <t>1248</t>
-  </si>
-  <si>
-    <t>2020-04-28</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>14100.0</t>
-  </si>
-  <si>
-    <t>24-04-2020 11:30:40</t>
-  </si>
-  <si>
-    <t>1700</t>
-  </si>
-  <si>
-    <t>24-04-2020 11:57:44</t>
-  </si>
-  <si>
-    <t>1062</t>
-  </si>
-  <si>
-    <t>24-04-2020 12:10:54</t>
-  </si>
-  <si>
-    <t>1715</t>
-  </si>
-  <si>
-    <t>24-04-2020 12:14:04</t>
-  </si>
-  <si>
-    <t>1041</t>
-  </si>
-  <si>
-    <t>24-04-2020 12:48:27</t>
-  </si>
-  <si>
-    <t>1719</t>
+    <t>2020-04-27</t>
+  </si>
+  <si>
+    <t>19700.0</t>
+  </si>
+  <si>
+    <t>24-04-2020 03:32:19</t>
+  </si>
+  <si>
+    <t>1573</t>
   </si>
 </sst>
 </file>
@@ -296,28 +263,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.65625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.91796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.4609375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.484375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.26171875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.25390625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.86328125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.6171875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.47265625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="7.0703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.49609375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="7.8046875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.66796875" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -468,13 +418,13 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
@@ -483,7 +433,7 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -492,36 +442,36 @@
         <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
         <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
@@ -530,7 +480,7 @@
         <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -545,13 +495,13 @@
         <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
         <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -559,13 +509,13 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -577,45 +527,45 @@
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" t="s">
         <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
         <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
         <v>27</v>
       </c>
       <c r="O6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
@@ -624,7 +574,7 @@
         <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
         <v>23</v>
@@ -639,33 +589,33 @@
         <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N7" t="s">
         <v>27</v>
       </c>
       <c r="O7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>21</v>
@@ -680,33 +630,33 @@
         <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L8" t="s">
         <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N8" t="s">
         <v>27</v>
       </c>
       <c r="O8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -727,36 +677,36 @@
         <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L9" t="s">
         <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N9" t="s">
         <v>27</v>
       </c>
       <c r="O9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
         <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>33</v>
@@ -765,7 +715,7 @@
         <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="I10" t="s">
         <v>23</v>
@@ -777,33 +727,33 @@
         <v>25</v>
       </c>
       <c r="L10" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
         <v>27</v>
       </c>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
@@ -812,7 +762,7 @@
         <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s">
         <v>22</v>
@@ -827,27 +777,27 @@
         <v>25</v>
       </c>
       <c r="M11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N11" t="s">
         <v>27</v>
       </c>
       <c r="O11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -862,7 +812,7 @@
         <v>22</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s">
         <v>24</v>
@@ -871,204 +821,16 @@
         <v>25</v>
       </c>
       <c r="L12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" t="n">
-        <v>9900.0</v>
+        <v>25</v>
+      </c>
+      <c r="M12" t="s">
+        <v>66</v>
       </c>
       <c r="N12" t="s">
         <v>27</v>
       </c>
       <c r="O12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" t="n">
-        <v>6600.0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" t="n">
-        <v>6600.0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" t="n">
-        <v>24300.0</v>
-      </c>
-      <c r="N15" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" t="n">
-        <v>24300.0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>